<commit_message>
updated the structure and content
</commit_message>
<xml_diff>
--- a/data/raw_data/exampledata.xlsx
+++ b/data/raw_data/exampledata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FA2285-62C7-443A-BFBC-77E0754551CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFEB904-A6A1-4B5A-B8D7-ACD57168FEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="780" windowWidth="47655" windowHeight="21570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>Height</t>
   </si>
@@ -29,6 +29,18 @@
   </si>
   <si>
     <t>sixty</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -346,129 +358,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>180</v>
       </c>
       <c r="B2">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>175</v>
       </c>
       <c r="B3">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>178</v>
       </c>
       <c r="B5">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>192</v>
       </c>
       <c r="B6">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>156</v>
       </c>
       <c r="B8">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>166</v>
       </c>
       <c r="B9">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>155</v>
       </c>
       <c r="B10">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>145</v>
       </c>
       <c r="B11">
         <v>7000</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>165</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>133</v>
       </c>
       <c r="B13">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>166</v>
       </c>
       <c r="B14">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>154</v>
       </c>
       <c r="B15">
         <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates, still needs checking
</commit_message>
<xml_diff>
--- a/data/raw_data/exampledata.xlsx
+++ b/data/raw_data/exampledata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F6676E-8A84-4027-81F4-2285066F9254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="420" windowWidth="44640" windowHeight="21645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="945" windowWidth="48840" windowHeight="21645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Height</t>
   </si>
@@ -32,9 +32,6 @@
     <t>sixty</t>
   </si>
   <si>
-    <t>Sex</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -50,13 +47,31 @@
     <t>Variable Definition</t>
   </si>
   <si>
-    <t>biological sex</t>
-  </si>
-  <si>
     <t>weight in kilograms</t>
   </si>
   <si>
     <t>height in centimeters</t>
+  </si>
+  <si>
+    <t>Allowed Values</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>numeric value &gt;0 or NA</t>
+  </si>
+  <si>
+    <t>M/F/O/NA</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>identified gender (male/female/other)</t>
   </si>
 </sst>
 </file>
@@ -386,7 +401,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +414,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -410,7 +425,7 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -421,7 +436,7 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -432,7 +447,7 @@
         <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -443,7 +458,7 @@
         <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -454,7 +469,7 @@
         <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -465,7 +480,7 @@
         <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -476,7 +491,7 @@
         <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -487,7 +502,7 @@
         <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -498,7 +513,7 @@
         <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -509,7 +524,7 @@
         <v>7000</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -517,7 +532,7 @@
         <v>165</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,7 +543,7 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -539,7 +554,7 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -550,7 +565,7 @@
         <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -560,48 +575,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>